<commit_message>
RM Payment and RM bils
</commit_message>
<xml_diff>
--- a/src/assets/templates/Sample_format_BillerBulk_Para1.xlsx
+++ b/src/assets/templates/Sample_format_BillerBulk_Para1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="179">
   <si>
     <t>Discom_Name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Dakshin Gujarat Vij</t>
   </si>
   <si>
-    <t>149825585</t>
-  </si>
-  <si>
     <t>Gujarat</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>Hubli Electricity  (HESCOM)</t>
   </si>
   <si>
-    <t>110083094</t>
-  </si>
-  <si>
     <t>167491309</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
     <t>Jamshedpur Utilities (JUSCO)</t>
   </si>
   <si>
-    <t>81620006</t>
-  </si>
-  <si>
     <t>Jharkhand</t>
   </si>
   <si>
@@ -306,9 +297,6 @@
     <t>Kerala State Electricity(KSEB)</t>
   </si>
   <si>
-    <t>81221328</t>
-  </si>
-  <si>
     <t>Kerala</t>
   </si>
   <si>
@@ -327,9 +315,6 @@
     <t>209808766</t>
   </si>
   <si>
-    <t>149825584</t>
-  </si>
-  <si>
     <t xml:space="preserve">Madhya Pradesh Paschim Kshetra </t>
   </si>
   <si>
@@ -387,9 +372,6 @@
     <t>Noida Power Company Ltd (NPCL)</t>
   </si>
   <si>
-    <t>92897779</t>
-  </si>
-  <si>
     <t>25534742</t>
   </si>
   <si>
@@ -405,21 +387,12 @@
     <t>CA Number/CON ID</t>
   </si>
   <si>
-    <t>21245756</t>
-  </si>
-  <si>
-    <t>Connection ID</t>
-  </si>
-  <si>
     <t>Paschim Gujarat Vij</t>
   </si>
   <si>
     <t>209809553</t>
   </si>
   <si>
-    <t>149825583</t>
-  </si>
-  <si>
     <t>Punjab State Power (PSPCL)</t>
   </si>
   <si>
@@ -453,9 +426,6 @@
     <t>243209306</t>
   </si>
   <si>
-    <t>21674295</t>
-  </si>
-  <si>
     <t>SOUTHCO, Odhisha</t>
   </si>
   <si>
@@ -510,9 +480,6 @@
     <t>209809881</t>
   </si>
   <si>
-    <t>149825586</t>
-  </si>
-  <si>
     <t>Uttar Haryana Bijli (UHBVN)</t>
   </si>
   <si>
@@ -580,6 +547,12 @@
   </si>
   <si>
     <t>Enter Contact No here</t>
+  </si>
+  <si>
+    <t>Adani Electricity</t>
+  </si>
+  <si>
+    <t>Power &amp; Electricity Department - Mizoram</t>
   </si>
 </sst>
 </file>
@@ -929,16 +902,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -962,28 +935,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1000,25 +973,25 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1035,25 +1008,25 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1070,25 +1043,25 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1105,25 +1078,25 @@
         <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1140,25 +1113,25 @@
         <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1175,25 +1148,25 @@
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1210,25 +1183,25 @@
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1245,30 +1218,30 @@
         <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
@@ -1280,25 +1253,25 @@
         <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1315,25 +1288,25 @@
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1350,25 +1323,25 @@
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1385,25 +1358,25 @@
         <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1420,25 +1393,25 @@
         <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1455,25 +1428,25 @@
         <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1490,25 +1463,25 @@
         <v>50</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1516,427 +1489,427 @@
         <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
@@ -1945,103 +1918,103 @@
         <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
@@ -2050,1320 +2023,970 @@
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="1" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>127</v>
+        <v>11</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="1" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="1" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>127</v>
+        <v>52</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="1" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>12</v>
+        <v>159</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="1" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K60" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
-      <c r="A65" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
-      <c r="A66" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K66" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
-      <c r="A67" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
-      <c r="A68" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
-      <c r="A69" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>